<commit_message>
Run experiment with outliers (p=0,25%)
</commit_message>
<xml_diff>
--- a/Results/Plots/A_10_Noiseless_with_chart.xlsx
+++ b/Results/Plots/A_10_Noiseless_with_chart.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AAA_UNIV\MAI\MP\Codebase\LSTM_Periodic_Function\Results\Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2968383-50BB-4523-B113-01878F1F8C76}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30BF412-9FFA-4A49-9E53-5C418BD95400}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1508,6 +1509,60 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Outliers (P=0.0025)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>('[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$3,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$5,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$7,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$9,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$11,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4474629610776901E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.02550207078456E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.58301194012165E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1279861479997599E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.04959697462618E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2417553365230498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46AD-469F-9DEA-6867051A0374}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1602,7 +1657,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('[4]A_10_Outliers_P_10_L_4_M_2,3'!$E$3,'[4]A_10_Outliers_P_10_L_4_M_2,3'!$E$5,'[4]A_10_Outliers_P_10_L_4_M_2,3'!$E$7,'[4]A_10_Outliers_P_10_L_4_M_2,3'!$E$9,'[4]A_10_Outliers_P_10_L_4_M_2,3'!$E$11,'[4]A_10_Outliers_P_10_L_4_M_2,3'!$E$13)</c15:sqref>
@@ -1634,7 +1689,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-6246-4E61-8E41-B552FED62496}"/>
                   </c:ext>
@@ -1662,7 +1717,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>([5]A_10_Gaussian_2_Disturbing_F_2_!$E$3,[5]A_10_Gaussian_2_Disturbing_F_2_!$E$5,[5]A_10_Gaussian_2_Disturbing_F_2_!$E$7,[5]A_10_Gaussian_2_Disturbing_F_2_!$E$9,[5]A_10_Gaussian_2_Disturbing_F_2_!$E$11,[5]A_10_Gaussian_2_Disturbing_F_2_!$E$13)</c15:sqref>
@@ -1694,7 +1749,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-6246-4E61-8E41-B552FED62496}"/>
                   </c:ext>
@@ -2557,7 +2612,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
@@ -2853,6 +2908,50 @@
         <row r="13">
           <cell r="E13">
             <v>0.34835886955261203</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="A_10_Outliers_P_0,25_L_4_M_3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3">
+            <v>1.4474629610776901E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>2.02550207078456E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>4.58301194012165E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>1.1279861479997599E-2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>1.04959697462618E-3</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>2.2417553365230498E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -3157,11 +3256,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated graphs with recent experiments
</commit_message>
<xml_diff>
--- a/Results/Plots/A_10_Noiseless_with_chart.xlsx
+++ b/Results/Plots/A_10_Noiseless_with_chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AAA_UNIV\MAI\MP\Codebase\LSTM_Periodic_Function\Results\Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30BF412-9FFA-4A49-9E53-5C418BD95400}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868CE0C6-C412-4E01-B4EC-AE764B11AD74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,10 @@
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
@@ -1406,58 +1410,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Gaussian (dev 0.2)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>([1]A_10_Gaussian_02!$E$3,[1]A_10_Gaussian_02!$E$5,[1]A_10_Gaussian_02!$E$7,[1]A_10_Gaussian_02!$E$9,[1]A_10_Gaussian_02!$E$11,[1]A_10_Gaussian_02!$E$13)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.4540212303400005E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.16183152608573E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.85826209187507E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.09080316126346E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.8242052067071199E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6873018592595999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-6246-4E61-8E41-B552FED62496}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
@@ -1510,15 +1462,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:idx val="7"/>
+          <c:order val="7"/>
           <c:tx>
-            <c:v>Outliers (P=0.0025)</c:v>
+            <c:v>Disturbing F increasing A (f=2, A=0.001 t + 0.5)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -1531,27 +1483,27 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>('[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$3,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$5,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$7,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$9,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$11,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$13)</c:f>
+              <c:f>('[7]A_10_Increasing_Amp_a_0,001_b_0'!$E$3,'[7]A_10_Increasing_Amp_a_0,001_b_0'!$E$5,'[7]A_10_Increasing_Amp_a_0,001_b_0'!$E$7,'[7]A_10_Increasing_Amp_a_0,001_b_0'!$E$9,'[7]A_10_Increasing_Amp_a_0,001_b_0'!$E$11,'[7]A_10_Increasing_Amp_a_0,001_b_0'!$E$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4474629610776901E-2</c:v>
+                  <c:v>5.5682915262877898E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.02550207078456E-2</c:v>
+                  <c:v>5.2556283771991704E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.58301194012165E-2</c:v>
+                  <c:v>7.2132633067667398E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1279861479997599E-2</c:v>
+                  <c:v>3.3008144237101002E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.04959697462618E-3</c:v>
+                  <c:v>7.2681535966694303E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2417553365230498E-2</c:v>
+                  <c:v>5.0550815649330605E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,7 +1511,61 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-46AD-469F-9DEA-6867051A0374}"/>
+              <c16:uniqueId val="{00000000-A8AD-4EAC-A3DD-7BD628C05A30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Disturbing F increasing F (f=0.01t+0.001, A=3)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>('[9]A_10_Increasing_Freq_a_0,01_b_0'!$E$3,'[9]A_10_Increasing_Freq_a_0,01_b_0'!$E$5,'[9]A_10_Increasing_Freq_a_0,01_b_0'!$E$7,'[9]A_10_Increasing_Freq_a_0,01_b_0'!$E$9,'[9]A_10_Increasing_Freq_a_0,01_b_0'!$E$11,'[9]A_10_Increasing_Freq_a_0,01_b_0'!$E$13)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.2368200421333296E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3592378944158499E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8328701853752102E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8359697684645601E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1693753767758599E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.07987336814403E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A8AD-4EAC-A3DD-7BD628C05A30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1576,6 +1582,66 @@
         <c:axId val="427788480"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>Gaussian (dev 0.2)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>([1]A_10_Gaussian_02!$E$3,[1]A_10_Gaussian_02!$E$5,[1]A_10_Gaussian_02!$E$7,[1]A_10_Gaussian_02!$E$9,[1]A_10_Gaussian_02!$E$11,[1]A_10_Gaussian_02!$E$13)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>9.4540212303400005E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3.16183152608573E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.85826209187507E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2.09080316126346E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2.8242052067071199E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.6873018592595999E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-6246-4E61-8E41-B552FED62496}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
             <c15:filteredLineSeries>
               <c15:ser>
                 <c:idx val="2"/>
@@ -1597,8 +1663,8 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>([2]A_10_Gaussian_1!$E$3,[2]A_10_Gaussian_1!$E$5,[2]A_10_Gaussian_1!$E$7,[2]A_10_Gaussian_1!$E$9,[2]A_10_Gaussian_1!$E$11,[2]A_10_Gaussian_1!$E$13)</c15:sqref>
                         </c15:formulaRef>
@@ -1629,7 +1695,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-6246-4E61-8E41-B552FED62496}"/>
                   </c:ext>
@@ -1752,6 +1818,192 @@
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-6246-4E61-8E41-B552FED62496}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:tx>
+                  <c:v>Outliers (P=0.0025)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$3,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$5,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$7,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$9,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$11,'[6]A_10_Outliers_P_0,25_L_4_M_3'!$E$13)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1.4474629610776901E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.02550207078456E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.58301194012165E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.1279861479997599E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.04959697462618E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.2417553365230498E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-46AD-469F-9DEA-6867051A0374}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="8"/>
+                <c:order val="8"/>
+                <c:tx>
+                  <c:v>Disturbing F increasing A (f=2, A=0.1 t + 0.5)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('[8]A_10_Increasing_Amp_a_0,1_b_0,5'!$E$3,'[8]A_10_Increasing_Amp_a_0,1_b_0,5'!$E$5,'[8]A_10_Increasing_Amp_a_0,1_b_0,5'!$E$7,'[8]A_10_Increasing_Amp_a_0,1_b_0,5'!$E$9,'[8]A_10_Increasing_Amp_a_0,1_b_0,5'!$E$11,'[8]A_10_Increasing_Amp_a_0,1_b_0,5'!$E$13)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>8.8299028575420293E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.37792015448212E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.5073902010917601E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.57049130648374E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5.1957345567643599E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.4473889023065499E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-A8AD-4EAC-A3DD-7BD628C05A30}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="10"/>
+                <c:order val="10"/>
+                <c:tx>
+                  <c:v>Disturbing F increasing A and F (f=0.01t + 0.001, A=t + 0.001)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('[10]A_10_Increasing_Amp_a_1_b_0,001'!$E$3,'[10]A_10_Increasing_Amp_a_1_b_0,001'!$E$5,'[10]A_10_Increasing_Amp_a_1_b_0,001'!$E$7,'[10]A_10_Increasing_Amp_a_1_b_0,001'!$E$9,'[10]A_10_Increasing_Amp_a_1_b_0,001'!$E$11,'[10]A_10_Increasing_Amp_a_1_b_0,001'!$E$13)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>5.86383156478405E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.25929298996925298</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.0195001736283299E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.182126954197883</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.126170843839645</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.113061673939228</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-A8AD-4EAC-A3DD-7BD628C05A30}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -2740,6 +2992,50 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="A_10_Increasing_Amp_a_1_b_0,001"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3">
+            <v>5.86383156478405E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>0.25929298996925298</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>2.0195001736283299E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>0.182126954197883</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>0.126170843839645</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>0.113061673939228</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -2952,6 +3248,138 @@
         <row r="13">
           <cell r="E13">
             <v>2.2417553365230498E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="A_10_Increasing_Amp_a_0,001_b_0"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3">
+            <v>5.5682915262877898E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>5.2556283771991704E-3</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>7.2132633067667398E-3</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>3.3008144237101002E-4</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>7.2681535966694303E-3</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>5.0550815649330605E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="A_10_Increasing_Amp_a_0,1_b_0,5"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3">
+            <v>8.8299028575420293E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>1.37792015448212E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>5.5073902010917601E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>1.57049130648374E-2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>5.1957345567643599E-3</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>1.4473889023065499E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="A_10_Increasing_Freq_a_0,01_b_0"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3">
+            <v>9.2368200421333296E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>2.3592378944158499E-2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>2.8328701853752102E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>4.8359697684645601E-3</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>1.1693753767758599E-3</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>1.07987336814403E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -3259,8 +3687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AH27" sqref="AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>